<commit_message>
Updated references, cross references etc
</commit_message>
<xml_diff>
--- a/supplementary-material/inputs/excluded_studies.xlsx
+++ b/supplementary-material/inputs/excluded_studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtay0016/dev/youth-homelessness-review/supplementary-material/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73E8338-8938-474C-947C-472C05B30EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABF8D4E-B2F6-674D-9881-D6EFA2CDDF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{553D8D9E-65D0-C741-9498-31108965572F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{553D8D9E-65D0-C741-9498-31108965572F}"/>
   </bookViews>
   <sheets>
     <sheet name="excluded" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>dore-gauthier2020specializedassertivecommunity</t>
   </si>
   <si>
-    <t>smith1996eighteenmonthfollowdatatreatment</t>
-  </si>
-  <si>
     <t>ocampo2017foodsecurityindividuals</t>
   </si>
   <si>
@@ -372,6 +369,9 @@
   </si>
   <si>
     <t>Rationale</t>
+  </si>
+  <si>
+    <t>smith1996eighteenmonthfollowupdata</t>
   </si>
 </sst>
 </file>
@@ -435,13 +435,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -782,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4766544E-77F8-5148-AF8F-2048DE2C7546}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,18 +800,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>75</v>
+      <c r="C2" t="s">
+        <v>74</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -820,14 +819,14 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>86</v>
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -835,14 +834,14 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>86</v>
+      <c r="C4" t="s">
+        <v>85</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -850,14 +849,14 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>102</v>
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -865,14 +864,14 @@
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>86</v>
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -880,14 +879,14 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>86</v>
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -895,14 +894,14 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>103</v>
+      <c r="C8" t="s">
+        <v>102</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -910,14 +909,14 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>86</v>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -925,14 +924,14 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>95</v>
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -940,14 +939,14 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>104</v>
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -955,14 +954,14 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>105</v>
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -970,14 +969,14 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>106</v>
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>105</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -985,14 +984,14 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>86</v>
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1000,14 +999,14 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>86</v>
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1015,14 +1014,14 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>108</v>
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>107</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1030,14 +1029,14 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>107</v>
+      <c r="C17" t="s">
+        <v>106</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1045,14 +1044,14 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>87</v>
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1060,14 +1059,14 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>109</v>
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>108</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1075,14 +1074,14 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>110</v>
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1090,14 +1089,14 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>86</v>
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>85</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1105,14 +1104,14 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>101</v>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1120,14 +1119,14 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>86</v>
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1135,14 +1134,14 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>86</v>
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1150,14 +1149,14 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>86</v>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>85</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1165,14 +1164,14 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>76</v>
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1180,14 +1179,14 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>79</v>
+      <c r="C27" t="s">
+        <v>78</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1195,14 +1194,14 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>21</v>
+      <c r="A28" t="s">
+        <v>20</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>86</v>
+      <c r="C28" t="s">
+        <v>85</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1210,14 +1209,14 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>30</v>
+      <c r="A29" t="s">
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>86</v>
+      <c r="C29" t="s">
+        <v>85</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1231,8 +1230,8 @@
       <c r="B30" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>86</v>
+      <c r="C30" t="s">
+        <v>85</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1240,14 +1239,14 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>86</v>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>85</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1255,14 +1254,14 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>86</v>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1270,14 +1269,14 @@
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>86</v>
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>85</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1285,14 +1284,14 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>100</v>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>99</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1300,14 +1299,14 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>86</v>
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>85</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1315,14 +1314,14 @@
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>99</v>
+      <c r="C36" t="s">
+        <v>98</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1330,14 +1329,14 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>94</v>
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1345,14 +1344,14 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>86</v>
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1360,14 +1359,14 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>86</v>
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1375,14 +1374,14 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>86</v>
+      <c r="A40" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1390,14 +1389,14 @@
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>84</v>
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1405,14 +1404,14 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>78</v>
+      <c r="C42" t="s">
+        <v>77</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1420,14 +1419,14 @@
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>98</v>
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>97</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1435,14 +1434,14 @@
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="3" t="s">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>85</v>
+      <c r="C44" t="s">
+        <v>84</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1450,14 +1449,14 @@
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>96</v>
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>95</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1465,14 +1464,14 @@
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>97</v>
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>96</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -1480,14 +1479,14 @@
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>88</v>
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1495,14 +1494,14 @@
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="3" t="s">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>82</v>
+      <c r="C48" t="s">
+        <v>81</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1510,14 +1509,14 @@
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="A49" t="s">
         <v>68</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>67</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -1525,14 +1524,14 @@
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" s="3" t="s">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>82</v>
+      <c r="C50" t="s">
+        <v>81</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1540,14 +1539,14 @@
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>89</v>
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>88</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1555,14 +1554,14 @@
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>93</v>
+      <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>92</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1570,14 +1569,14 @@
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>83</v>
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>82</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -1585,14 +1584,14 @@
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>82</v>
+      <c r="C54" t="s">
+        <v>81</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1600,14 +1599,14 @@
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B55" s="5" t="s">
+      <c r="A55" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>75</v>
+      <c r="C55" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -1615,14 +1614,14 @@
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>78</v>
+      <c r="C56" t="s">
+        <v>77</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -1630,14 +1629,14 @@
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>90</v>
+      <c r="A57" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>89</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -1645,14 +1644,14 @@
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>91</v>
+      <c r="A58" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>90</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -1660,14 +1659,14 @@
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>92</v>
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>91</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -1675,14 +1674,14 @@
       <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="3" t="s">
+      <c r="A60" t="s">
         <v>72</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>71</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -1690,14 +1689,14 @@
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
+      <c r="A61" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>80</v>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>79</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -1705,14 +1704,14 @@
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>86</v>
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>85</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -1720,14 +1719,14 @@
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>86</v>
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -1735,14 +1734,14 @@
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>86</v>
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>85</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -1750,14 +1749,14 @@
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>86</v>
+      <c r="A65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>85</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -1765,14 +1764,14 @@
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>86</v>
+      <c r="A66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>85</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -1780,14 +1779,14 @@
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="3" t="s">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>77</v>
+      <c r="C67" t="s">
+        <v>76</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -1795,14 +1794,14 @@
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>81</v>
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>80</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -1810,15 +1809,15 @@
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="4"/>
-      <c r="C70" s="6"/>
+      <c r="A70" s="3"/>
+      <c r="C70" s="5"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B75" s="4"/>
+      <c r="B75" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>